<commit_message>
use case description edits
</commit_message>
<xml_diff>
--- a/SSYSADD1 DOCU/Diagrams/Use Case Description(new).xlsx
+++ b/SSYSADD1 DOCU/Diagrams/Use Case Description(new).xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="77">
   <si>
     <t>Use Case</t>
   </si>
@@ -131,6 +131,9 @@
     <t>2. Patient inserts new time and/or date of the appointment</t>
   </si>
   <si>
+    <t>Dermatologist</t>
+  </si>
+  <si>
     <t>2.1. System will check the dermatologists availability (if within operating hours)</t>
   </si>
   <si>
@@ -218,9 +221,6 @@
     <t>4.  Email Authentication</t>
   </si>
   <si>
-    <t>4.1. System will send an email authentication using the email input in basic data. (1.1.)</t>
-  </si>
-  <si>
     <t>5. Sucessful Registration</t>
   </si>
   <si>
@@ -234,6 +234,27 @@
   </si>
   <si>
     <t>If the dermatologist did not confirm the appointment, the appointment will be cancelled; sending an invitation to both parties that the appointment invite expired.</t>
+  </si>
+  <si>
+    <t>4.1. System will send an email authentication using the email input in basic data. (System activity 1.1.)</t>
+  </si>
+  <si>
+    <t>Insert Appointment Details</t>
+  </si>
+  <si>
+    <t>Dermatologist will record the events for the accomplished appointment</t>
+  </si>
+  <si>
+    <t>Accomplished appointment</t>
+  </si>
+  <si>
+    <t>Accomplished Appointment</t>
+  </si>
+  <si>
+    <t>The dermatologist will make a summary of all the necessary details and information on the accomplished appointment</t>
+  </si>
+  <si>
+    <t>Dermatologist, Patient</t>
   </si>
 </sst>
 </file>
@@ -770,8 +791,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C115"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C33" sqref="C33"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1021,14 +1042,14 @@
         <v>34</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="13"/>
       <c r="B30" s="8"/>
       <c r="C30" s="3" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1057,7 +1078,7 @@
         <v>0</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C35" s="5"/>
     </row>
@@ -1066,7 +1087,7 @@
         <v>1</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C36" s="5"/>
     </row>
@@ -1075,7 +1096,7 @@
         <v>2</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C37" s="5"/>
     </row>
@@ -1084,7 +1105,7 @@
         <v>3</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C38" s="5"/>
     </row>
@@ -1102,7 +1123,7 @@
         <v>5</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C40" s="5"/>
     </row>
@@ -1120,7 +1141,7 @@
         <v>7</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C42" s="5"/>
     </row>
@@ -1129,7 +1150,7 @@
         <v>8</v>
       </c>
       <c r="B43" s="17" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C43" s="18"/>
     </row>
@@ -1147,31 +1168,31 @@
     <row r="45" spans="1:3" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="15"/>
       <c r="B45" s="3" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="15"/>
       <c r="B46" s="3"/>
       <c r="C46" s="3" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="47" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A47" s="15"/>
       <c r="B47" s="3"/>
       <c r="C47" s="3" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="48" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A48" s="16"/>
       <c r="B48" s="3"/>
       <c r="C48" s="3" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="49" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1187,7 +1208,7 @@
         <v>0</v>
       </c>
       <c r="B52" s="20" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C52" s="21"/>
     </row>
@@ -1196,7 +1217,7 @@
         <v>1</v>
       </c>
       <c r="B53" s="20" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C53" s="21"/>
     </row>
@@ -1205,7 +1226,7 @@
         <v>2</v>
       </c>
       <c r="B54" s="20" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C54" s="21"/>
     </row>
@@ -1214,7 +1235,7 @@
         <v>3</v>
       </c>
       <c r="B55" s="20" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C55" s="21"/>
     </row>
@@ -1223,7 +1244,7 @@
         <v>4</v>
       </c>
       <c r="B56" s="20" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C56" s="21"/>
     </row>
@@ -1232,7 +1253,7 @@
         <v>5</v>
       </c>
       <c r="B57" s="20" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C57" s="21"/>
     </row>
@@ -1241,7 +1262,7 @@
         <v>6</v>
       </c>
       <c r="B58" s="20" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C58" s="21"/>
     </row>
@@ -1257,7 +1278,7 @@
         <v>8</v>
       </c>
       <c r="B60" s="22" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C60" s="23"/>
     </row>
@@ -1275,37 +1296,37 @@
     <row r="62" spans="1:3" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="15"/>
       <c r="B62" s="24" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C62" s="24" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row r="63" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A63" s="15"/>
       <c r="B63" s="24" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C63" s="24" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
     <row r="64" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A64" s="15"/>
       <c r="B64" s="24" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C64" s="24" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
     </row>
     <row r="65" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A65" s="15"/>
       <c r="B65" s="24" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C65" s="24" t="s">
-        <v>64</v>
+        <v>70</v>
       </c>
     </row>
     <row r="66" spans="1:3" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1329,35 +1350,45 @@
       <c r="A70" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B70" s="20"/>
+      <c r="B70" s="20" t="s">
+        <v>71</v>
+      </c>
       <c r="C70" s="21"/>
     </row>
     <row r="71" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A71" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B71" s="20"/>
+      <c r="B71" s="20" t="s">
+        <v>72</v>
+      </c>
       <c r="C71" s="21"/>
     </row>
     <row r="72" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A72" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B72" s="20"/>
+      <c r="B72" s="20" t="s">
+        <v>73</v>
+      </c>
       <c r="C72" s="21"/>
     </row>
-    <row r="73" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:3" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A73" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B73" s="20"/>
+      <c r="B73" s="20" t="s">
+        <v>75</v>
+      </c>
       <c r="C73" s="21"/>
     </row>
     <row r="74" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A74" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B74" s="20"/>
+      <c r="B74" s="20" t="s">
+        <v>35</v>
+      </c>
       <c r="C74" s="21"/>
     </row>
     <row r="75" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1371,14 +1402,18 @@
       <c r="A76" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B76" s="20"/>
+      <c r="B76" s="20" t="s">
+        <v>76</v>
+      </c>
       <c r="C76" s="21"/>
     </row>
     <row r="77" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A77" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B77" s="20"/>
+      <c r="B77" s="20" t="s">
+        <v>74</v>
+      </c>
       <c r="C77" s="21"/>
     </row>
     <row r="78" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">

</xml_diff>